<commit_message>
remove actor.py - not used
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:F1048576"/>
@@ -846,9 +846,6 @@
       <c r="B11" t="n">
         <v>11</v>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve">                                        original_title  year                      genre language      budget  duration usa_gross_income  reviews_from_users
@@ -870,6 +867,51 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Olga</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>29</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                 original_title  year  genre language      budget  duration usa_gross_income  reviews_from_users
+31327            Ricochet River  2001  Drama  English         NaN       112              NaN                 7.0
+31335         The Shipping News  2001  Drama  English  $ 38000000       111       $ 11434216               210.0
+34751      The Invisible Circus  2001  Drama  English         NaN        93          $ 77578                49.0
+35164  A Day in Black and White  2001  Drama  English         NaN        80              NaN                 4.0
+36026          The Rising Place  2001  Drama  English         NaN        93           $ 8360                 2.0
+36414       The Sleepy Time Gal  2001  Drama  English         NaN       108              NaN                14.0
+36460    Diary of a City Priest  2001  Drama  English         NaN        77              NaN                 4.0
+36705           Sensual Friends  2001  Drama  English         NaN        93              NaN                 6.0
+36899    Goodbye Charlie Bright  2001  Drama  English         NaN        87              NaN                24.0
+37077         Borderline Normal  2001  Drama  English         NaN        85              NaN                 8.0</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>